<commit_message>
Pdf con la explicación del P32
</commit_message>
<xml_diff>
--- a/src/main/java/algestudiante/p32/P32_UO277876.xlsx
+++ b/src/main/java/algestudiante/p32/P32_UO277876.xlsx
@@ -8,16 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\infer\git\alg_AunonAndreaUO277876\src\main\java\algestudiante\p32\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC834D2E-4A86-4EB1-8FAE-2467D8F2551F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{460F1178-C294-4A8F-B5D3-9DF5103FC748}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{760BF4A0-4F21-48FC-9449-0A68ABD67C67}"/>
   </bookViews>
   <sheets>
     <sheet name="Inversiones" sheetId="5" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -78,10 +75,10 @@
     <t>Ranking6.txt</t>
   </si>
   <si>
-    <t>t(O(n2) (ms)</t>
+    <t>t(O(n2) (ms))</t>
   </si>
   <si>
-    <t>tO(nlogn) (ms)</t>
+    <t>tO(nlogn) (ms))</t>
   </si>
 </sst>
 </file>
@@ -1221,14 +1218,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>438150</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>87630</xdr:rowOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>49530</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>621030</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>87630</xdr:rowOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>49530</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1254,155 +1251,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="División"/>
-      <sheetName val="Sustracción"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1">
-        <row r="2">
-          <cell r="C2" t="str">
-            <v>t(sustracción1)</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="B3">
-            <v>1</v>
-          </cell>
-          <cell r="C3">
-            <v>8.9999999999999999E-8</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="B4">
-            <v>2</v>
-          </cell>
-          <cell r="C4">
-            <v>5.1159999999999998E-6</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="B5">
-            <v>4</v>
-          </cell>
-          <cell r="C5">
-            <v>1.2503E-5</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="B6">
-            <v>8</v>
-          </cell>
-          <cell r="C6">
-            <v>2.8138999999999999E-5</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="B7">
-            <v>16</v>
-          </cell>
-          <cell r="C7">
-            <v>5.6745E-5</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="B8">
-            <v>32</v>
-          </cell>
-          <cell r="C8">
-            <v>1.1825299999999999E-4</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="B9">
-            <v>64</v>
-          </cell>
-          <cell r="C9">
-            <v>1.3857999999999999E-4</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="B10">
-            <v>128</v>
-          </cell>
-          <cell r="C10">
-            <v>2.6158000000000003E-4</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="B11">
-            <v>256</v>
-          </cell>
-          <cell r="C11">
-            <v>5.6185000000000002E-4</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="B12">
-            <v>512</v>
-          </cell>
-          <cell r="C12">
-            <v>1.0606299999999999E-3</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="B13">
-            <v>1024</v>
-          </cell>
-          <cell r="C13">
-            <v>4.2931000000000002E-3</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="B14">
-            <v>2048</v>
-          </cell>
-          <cell r="C14">
-            <v>9.4696999999999993E-3</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="B15">
-            <v>4098</v>
-          </cell>
-          <cell r="C15">
-            <v>1.9399E-2</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="B16">
-            <v>8192</v>
-          </cell>
-          <cell r="C16">
-            <v>3.9403000000000001E-2</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="B17">
-            <v>16384</v>
-          </cell>
-          <cell r="C17">
-            <v>7.986E-2</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="B18">
-            <v>32768</v>
-          </cell>
-          <cell r="C18">
-            <v>0.16129099999999999</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1705,14 +1553,14 @@
   <dimension ref="A2:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19.21875" customWidth="1"/>
     <col min="2" max="2" width="14.21875" customWidth="1"/>
-    <col min="3" max="3" width="13.77734375" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" customWidth="1"/>
     <col min="4" max="4" width="18.21875" customWidth="1"/>
     <col min="5" max="5" width="19.77734375" customWidth="1"/>
     <col min="6" max="6" width="19.21875" customWidth="1"/>

</xml_diff>